<commit_message>
Stretched the columns in the data_combined Excel sheet.
</commit_message>
<xml_diff>
--- a/Apple_data_dividends.xlsx
+++ b/Apple_data_dividends.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B83"/>
+  <dimension ref="A1:B84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1105,6 +1105,14 @@
         <v>0.24</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" s="2" t="n">
+        <v>45422</v>
+      </c>
+      <c r="B84" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>